<commit_message>
updated with caps, resistors, inductors, and switches up to page 34
</commit_message>
<xml_diff>
--- a/pins.xlsx
+++ b/pins.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="16600" windowHeight="14160" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="16620" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1909,7 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F612"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
       <selection activeCell="H385" sqref="H385"/>
     </sheetView>
   </sheetViews>

</xml_diff>